<commit_message>
added standoffs and updated assembly
</commit_message>
<xml_diff>
--- a/pcb/bom.xlsx
+++ b/pcb/bom.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\Projects\mppc\4-Interface\mppcInterface\pcb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\Projects\mppcInterface\4-channel\mppcInterface\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$1</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="90">
   <si>
     <t>QTY</t>
   </si>
@@ -270,17 +270,45 @@
   </si>
   <si>
     <t>https://github.com/Sawaiz/mppcHighVoltage</t>
+  </si>
+  <si>
+    <t>Standoff Screws</t>
+  </si>
+  <si>
+    <t>M2.5 Size, 6mm Length, .45mm Pitch</t>
+  </si>
+  <si>
+    <t>92000A104</t>
+  </si>
+  <si>
+    <t>From McMaster</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#92000a104/=13ngkl7</t>
+  </si>
+  <si>
+    <t>Female Female Standoffs</t>
+  </si>
+  <si>
+    <t>4.5 mm Hex Size, 10 mm Length, M2.5 Thread Size</t>
+  </si>
+  <si>
+    <t>95947A005</t>
+  </si>
+  <si>
+    <t>http://www.mcmaster.com/#95947a005/=13ngfqz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,12 +322,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -330,21 +352,17 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -440,23 +458,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -492,23 +493,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -664,18 +648,18 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="93.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="5" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="98.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -693,13 +677,13 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -709,33 +693,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" t="s">
         <v>68</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="3">
-        <v>1</v>
-      </c>
-      <c r="F2" s="5">
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4">
         <v>6.3140000000000001</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="5">
         <v>10</v>
       </c>
       <c r="H2" s="1">
         <f>F2*G2</f>
         <v>63.14</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>66</v>
       </c>
     </row>
@@ -743,29 +727,29 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="4">
         <v>1.5129999999999999</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="5">
         <v>10</v>
       </c>
       <c r="H3" s="1">
         <f>F3*G3</f>
         <v>15.129999999999999</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -773,29 +757,29 @@
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="4">
         <v>0.184</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="5">
         <v>10</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" ref="H4" si="0">F4*G4</f>
         <v>1.8399999999999999</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -803,29 +787,29 @@
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="4">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
         <v>2.88</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="5">
         <v>10</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" ref="H5:H15" si="1">F5*G5</f>
         <v>28.799999999999997</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="6" t="s">
         <v>21</v>
       </c>
     </row>
@@ -833,29 +817,29 @@
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
         <v>0.98899999999999999</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="5">
         <v>10</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="1"/>
         <v>9.89</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -863,29 +847,29 @@
       <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
         <v>1.742</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="5">
         <v>10</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="1"/>
         <v>17.420000000000002</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="6" t="s">
         <v>35</v>
       </c>
     </row>
@@ -893,29 +877,29 @@
       <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="5">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
         <v>0.70199999999999996</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="5">
         <v>10</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
         <v>7.02</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -923,29 +907,29 @@
       <c r="A9" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="5">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
         <v>4.5199999999999996</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="5">
         <v>10</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="1"/>
         <v>45.199999999999996</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -953,119 +937,119 @@
       <c r="A10" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="5">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="5">
         <v>100</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="1"/>
         <v>0.37</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11">
         <v>2</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>3.3999999999999998E-3</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="5">
         <v>100</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
         <v>0.33999999999999997</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="5">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
         <v>4.7999999999999996E-3</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="5">
         <v>100</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
         <v>0.48</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4">
         <v>4.5999999999999999E-2</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="5">
         <v>50</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
         <v>2.2999999999999998</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="6" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1073,29 +1057,29 @@
       <c r="A14" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
-      <c r="F14" s="5">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4">
         <v>0.32600000000000001</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="5">
         <v>10</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
         <v>3.2600000000000002</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="6" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1103,29 +1087,29 @@
       <c r="A15" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" t="s">
         <v>75</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15">
         <v>2</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>0.28699999999999998</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="5">
         <v>10</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
         <v>2.8699999999999997</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="6" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1133,73 +1117,124 @@
       <c r="A16" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16">
         <v>4</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="I16" t="s">
+      <c r="I16" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E17" s="3"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E17"/>
       <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="2"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E18"/>
       <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E19" s="3"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E19"/>
       <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E20" s="3"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E21" s="3"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E22" s="3"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>3.44</v>
+      </c>
+      <c r="H20" s="7">
+        <v>3.44</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="G21" s="5">
+        <v>10</v>
+      </c>
+      <c r="H21" s="1">
+        <f>(F21*G21)</f>
+        <v>4.5</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E22" s="2"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E23" s="3"/>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E23" s="2"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E24" s="3"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E24" s="2"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E25" s="3"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E25" s="2"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E26" s="3"/>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E26" s="2"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E27" s="3"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E27" s="2"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E29" s="3"/>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E29" s="2"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="E30" s="3"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E30" s="2"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H32" s="1"/>
     </row>
   </sheetData>

</xml_diff>